<commit_message>
study update submodule update
</commit_message>
<xml_diff>
--- a/studies/compareScalingLaws_Dostal1981.xlsx
+++ b/studies/compareScalingLaws_Dostal1981.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="388">
   <si>
     <t>None</t>
   </si>
@@ -936,6 +936,240 @@
   </si>
   <si>
     <t>24.2 (10.8)</t>
+  </si>
+  <si>
+    <t>12.6 (5.6)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>3.8 (2.2)</t>
+  </si>
+  <si>
+    <t>4.2 (2.1)</t>
+  </si>
+  <si>
+    <t>4.1 (2.8)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>NonUniformLinearA</t>
+  </si>
+  <si>
+    <t>NonUniformLinearB</t>
+  </si>
+  <si>
+    <t>Pauwels2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>13.2 (21.0)</t>
+  </si>
+  <si>
+    <t>41.2 (33.6)</t>
+  </si>
+  <si>
+    <t>12.9 (29.1)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>4.2 (3.1)</t>
+  </si>
+  <si>
+    <t>3.2 (3.0)</t>
+  </si>
+  <si>
+    <t>3.8 (2.8)</t>
+  </si>
+  <si>
+    <t>Debrunner2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>24.9 (28.4)</t>
+  </si>
+  <si>
+    <t>12.6 (20.4)</t>
+  </si>
+  <si>
+    <t>23.1 (24.2)†</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>2.8 (3.0)</t>
+  </si>
+  <si>
+    <t>3.5 (3.6)</t>
+  </si>
+  <si>
+    <t>3.2 (3.0)</t>
+  </si>
+  <si>
+    <t>Iglic2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>23.0 (29.4)</t>
+  </si>
+  <si>
+    <t>16.5 (13.3)</t>
+  </si>
+  <si>
+    <t>20.1 (20.5)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>3.9 (2.8)</t>
+  </si>
+  <si>
+    <t>4.4 (5.0)</t>
+  </si>
+  <si>
+    <t>4.6 (2.4)</t>
+  </si>
+  <si>
+    <t>mediTEC2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>20.1 (24.0)</t>
+  </si>
+  <si>
+    <t>28.8 (22.9)</t>
+  </si>
+  <si>
+    <t>18.3 (18.2)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>3.9 (3.5)</t>
+  </si>
+  <si>
+    <t>4.6 (5.3)</t>
+  </si>
+  <si>
+    <t>4.7 (2.8)†</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>NonUniformLinearA</t>
+  </si>
+  <si>
+    <t>NonUniformLinearB</t>
+  </si>
+  <si>
+    <t>Pauwels2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>11.9 (27.1)</t>
+  </si>
+  <si>
+    <t>41.7 (14.5)†</t>
+  </si>
+  <si>
+    <t>17.5 (29.4)†</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>4.1 (3.3)</t>
+  </si>
+  <si>
+    <t>2.9 (3.6)</t>
+  </si>
+  <si>
+    <t>4.0 (3.6)</t>
+  </si>
+  <si>
+    <t>Debrunner2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>22.7 (23.3)</t>
+  </si>
+  <si>
+    <t>9.1 (19.0)</t>
+  </si>
+  <si>
+    <t>19.5 (18.8)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>4.3 (2.2)</t>
+  </si>
+  <si>
+    <t>3.6 (2.1)</t>
+  </si>
+  <si>
+    <t>4.5 (3.5)</t>
+  </si>
+  <si>
+    <t>Iglic2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>23.3 (20.9)</t>
+  </si>
+  <si>
+    <t>11.7 (10.9)</t>
+  </si>
+  <si>
+    <t>19.9 (19.6)</t>
+  </si>
+  <si>
+    <t>MAE Dir.</t>
+  </si>
+  <si>
+    <t>4.4 (2.4)</t>
+  </si>
+  <si>
+    <t>4.1 (2.0)</t>
+  </si>
+  <si>
+    <t>4.5 (3.8)†</t>
+  </si>
+  <si>
+    <t>mediTEC2021</t>
+  </si>
+  <si>
+    <t>MAE Mag.</t>
+  </si>
+  <si>
+    <t>14.6 (5.0)</t>
+  </si>
+  <si>
+    <t>24.3 (10.8)</t>
   </si>
   <si>
     <t>12.6 (5.6)</t>
@@ -985,7 +1219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1081,6 +1315,8 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
     <border/>
     <border/>
     <border/>
@@ -1091,7 +1327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -1125,6 +1361,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1430,134 +1668,134 @@
     <row r="2" s="2" customFormat="true">
       <c r="B2" s="1"/>
       <c r="C2" s="7" t="s">
-        <v>235</v>
+        <v>313</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
-        <v>244</v>
+        <v>322</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7" t="s">
-        <v>253</v>
+        <v>331</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="7" t="s">
-        <v>262</v>
+        <v>340</v>
       </c>
       <c r="J2" s="8"/>
     </row>
     <row r="3">
       <c r="B3" s="3"/>
       <c r="C3" s="9" t="s">
-        <v>236</v>
+        <v>314</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>240</v>
+        <v>318</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>245</v>
+        <v>323</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>249</v>
+        <v>327</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>254</v>
+        <v>332</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>258</v>
+        <v>336</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>263</v>
+        <v>341</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>267</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>232</v>
+        <v>310</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>237</v>
+        <v>315</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>241</v>
+        <v>319</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>246</v>
+        <v>324</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>250</v>
+        <v>328</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>255</v>
+        <v>333</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>259</v>
+        <v>337</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>264</v>
+        <v>342</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="3" t="s">
-        <v>233</v>
+        <v>311</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>238</v>
+        <v>316</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>242</v>
+        <v>320</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>247</v>
+        <v>325</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>251</v>
+        <v>329</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>256</v>
+        <v>334</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>260</v>
+        <v>338</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>265</v>
+        <v>343</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>269</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>234</v>
+        <v>312</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>239</v>
+        <v>317</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>248</v>
+        <v>326</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>252</v>
+        <v>330</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>257</v>
+        <v>335</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>261</v>
+        <v>339</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>266</v>
+        <v>344</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>270</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -1593,134 +1831,134 @@
     <row r="2" s="2" customFormat="true">
       <c r="B2" s="5"/>
       <c r="C2" s="7" t="s">
-        <v>274</v>
+        <v>352</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
-        <v>283</v>
+        <v>361</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7" t="s">
-        <v>292</v>
+        <v>370</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="13" t="s">
-        <v>301</v>
+        <v>379</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3">
       <c r="B3" s="6"/>
       <c r="C3" s="9" t="s">
-        <v>275</v>
+        <v>353</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>279</v>
+        <v>357</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>284</v>
+        <v>362</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>288</v>
+        <v>366</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>293</v>
+        <v>371</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>297</v>
+        <v>375</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>302</v>
+        <v>380</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>306</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="6" t="s">
-        <v>271</v>
+        <v>349</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>276</v>
+        <v>354</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>280</v>
+        <v>358</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>285</v>
+        <v>363</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>289</v>
+        <v>367</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>294</v>
+        <v>372</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>298</v>
+        <v>376</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>307</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="6" t="s">
-        <v>272</v>
+        <v>350</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>277</v>
+        <v>355</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>281</v>
+        <v>359</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>286</v>
+        <v>364</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>290</v>
+        <v>368</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>295</v>
+        <v>373</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>299</v>
+        <v>377</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>304</v>
+        <v>382</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>308</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="6" t="s">
-        <v>273</v>
+        <v>351</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>278</v>
+        <v>356</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>282</v>
+        <v>360</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>287</v>
+        <v>365</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>291</v>
+        <v>369</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>296</v>
+        <v>374</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>300</v>
+        <v>378</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>305</v>
+        <v>383</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>309</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>